<commit_message>
update billy exception list
</commit_message>
<xml_diff>
--- a/downloads/billy/billy_ausnahmeliste.xlsx
+++ b/downloads/billy/billy_ausnahmeliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\list\Documents\ocg-austria.github.io\downloads\billy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208C1350-888E-4473-87A4-93B4BEB7EF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B691B9-7917-4C3F-806F-B4983C05095A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="3150" windowWidth="23010" windowHeight="12210" xr2:uid="{B8557999-2838-4113-8C62-84179BA4D243}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="23010" windowHeight="12210" xr2:uid="{B8557999-2838-4113-8C62-84179BA4D243}"/>
   </bookViews>
   <sheets>
     <sheet name="Ausnahmen" sheetId="1" r:id="rId1"/>
@@ -36,40 +36,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Gregor Kölbl</author>
-  </authors>
-  <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{638601EB-D84C-403B-86E2-6B9EFED995C9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Gregor Kölbl:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Wann gilt die Regel NICHT?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
@@ -149,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,19 +135,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -682,12 +635,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDAE9F69-86AD-4FC8-9445-DA1FAD23C955}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDAE9F69-86AD-4FC8-9445-DA1FAD23C955}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1191,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1337,15 +1289,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101008291D1339C06284090D4ED3868DFF1D2" ma:contentTypeVersion="20" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="eccf34c2e58afab8dbe7b704ffe24f0a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="80225f2b-4a99-4030-98e8-1d936321691f" xmlns:ns3="e499901d-11da-4ecb-b3fa-a6aef8257c2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f41edb23db549c838e6164fb2bb857c6" ns2:_="" ns3:_="">
     <xsd:import namespace="80225f2b-4a99-4030-98e8-1d936321691f"/>
@@ -1614,6 +1557,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9197E329-3007-46C0-91C7-AB3E46A9121F}">
   <ds:schemaRefs>
@@ -1626,14 +1578,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3103435C-319A-493D-BBEB-26A8DF6B9E08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5050309-0478-4C57-9B34-55E2A464D94B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1650,4 +1594,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3103435C-319A-493D-BBEB-26A8DF6B9E08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>